<commit_message>
i do not know what happened
</commit_message>
<xml_diff>
--- a/data/place_export_2024-01-31.xlsx
+++ b/data/place_export_2024-01-31.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hac13/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prodduke-my.sharepoint.com/personal/am618_duke_edu/Documents/Mestyan_files/Github/CairoUrbanNews/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0546D299-7010-724E-AA93-3D5231C9E06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{0546D299-7010-724E-AA93-3D5231C9E06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67048FC1-6200-BC4D-98CD-310E3C8A1571}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="4660" windowWidth="26040" windowHeight="14940" xr2:uid="{57AA0200-3E71-B443-96E5-8D789C683223}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{57AA0200-3E71-B443-96E5-8D789C683223}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="places" localSheetId="0">Sheet1!$A$1:$E$2554</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25640,7 +25640,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25851,7 +25851,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>HYPERLINK(E10)</f>
         <v>https://project-cairo-urban-news.github.io/CairoUrbanNews/articles/arabic/1245.html#place-WA1245004701_03</v>
       </c>
     </row>

</xml_diff>